<commit_message>
New Calgem models, page order sorted
ISGS hole_size cleaning function correction
</commit_message>
<xml_diff>
--- a/processor_schemas/ISGS Well Completion Schema.xlsx
+++ b/processor_schemas/ISGS Well Completion Schema.xlsx
@@ -1263,10 +1263,10 @@
     <t>Ground</t>
   </si>
   <si>
+    <t>convert_hole_size_to_decimal</t>
+  </si>
+  <si>
     <t>Electric_Logs_Run_Date</t>
-  </si>
-  <si>
-    <t>convert_hole_size_to_decimal</t>
   </si>
   <si>
     <t>Water</t>
@@ -3841,7 +3841,7 @@
     <xdr:ext cx="2028825" cy="2762250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image9.png" title="Completion_A"/>
+        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image5.png" title="Completion_A"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3869,7 +3869,7 @@
     <xdr:ext cx="2009775" cy="2771775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Completion_C Page 1"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Completion_C Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3925,7 +3925,7 @@
     <xdr:ext cx="1981200" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image6.png" title="Competion_D Page 1"/>
+        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image4.png" title="Competion_D Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3953,7 +3953,7 @@
     <xdr:ext cx="1990725" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two variations of this format" id="0" name="image4.png" title="Completion_D Page 2"/>
+        <xdr:cNvPr descr="There are two variations of this format" id="0" name="image3.png" title="Completion_D Page 2"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3981,7 +3981,7 @@
     <xdr:ext cx="2047875" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Completion_E Page 1"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Completion_E Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4009,7 +4009,7 @@
     <xdr:ext cx="1952625" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Completion_E"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Completion_E"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4037,7 +4037,7 @@
     <xdr:ext cx="1762125" cy="2324100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4065,7 +4065,7 @@
     <xdr:ext cx="2581275" cy="2133600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5430,7 +5430,7 @@
         <v>401</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J31" s="24"/>
       <c r="K31" s="24"/>
@@ -7531,7 +7531,7 @@
         <v>401</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
@@ -9215,7 +9215,7 @@
         <v>401</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
@@ -9345,7 +9345,7 @@
         <v>401</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
@@ -9603,7 +9603,7 @@
         <v>401</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J27" s="31"/>
       <c r="K27" s="31"/>
@@ -9689,7 +9689,7 @@
         <v>401</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J29" s="31"/>
       <c r="K29" s="31"/>
@@ -9859,7 +9859,7 @@
         <v>401</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J33" s="31"/>
       <c r="K33" s="31"/>
@@ -9945,7 +9945,7 @@
         <v>401</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J35" s="31"/>
       <c r="K35" s="31"/>
@@ -10115,7 +10115,7 @@
         <v>401</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J39" s="31"/>
       <c r="K39" s="31"/>
@@ -10245,7 +10245,7 @@
         <v>401</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J41" s="31"/>
       <c r="K41" s="31"/>
@@ -10542,7 +10542,7 @@
         <v>401</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J46" s="30"/>
       <c r="K46" s="20" t="s">
@@ -14723,7 +14723,7 @@
         <v>401</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J60" s="30"/>
       <c r="K60" s="30"/>
@@ -17020,7 +17020,7 @@
         <v>401</v>
       </c>
       <c r="I44" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
@@ -17143,7 +17143,7 @@
         <v>401</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J47" s="31"/>
       <c r="K47" s="31"/>
@@ -17264,7 +17264,7 @@
         <v>401</v>
       </c>
       <c r="I50" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J50" s="30"/>
       <c r="K50" s="30"/>
@@ -17369,7 +17369,7 @@
         <v>401</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J53" s="31"/>
       <c r="K53" s="31"/>
@@ -17472,7 +17472,7 @@
         <v>401</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J56" s="30"/>
       <c r="K56" s="30"/>
@@ -17595,7 +17595,7 @@
         <v>401</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J59" s="31"/>
       <c r="K59" s="31"/>
@@ -19712,7 +19712,7 @@
         <v>401</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J41" s="31"/>
       <c r="K41" s="31"/>
@@ -19853,7 +19853,7 @@
         <v>401</v>
       </c>
       <c r="I44" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
@@ -19994,7 +19994,7 @@
         <v>401</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J47" s="31"/>
       <c r="K47" s="31"/>
@@ -20105,7 +20105,7 @@
         <v>401</v>
       </c>
       <c r="I50" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J50" s="30"/>
       <c r="K50" s="30"/>
@@ -20216,7 +20216,7 @@
         <v>401</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J53" s="31"/>
       <c r="K53" s="31"/>
@@ -20357,7 +20357,7 @@
         <v>401</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J56" s="30"/>
       <c r="K56" s="30"/>
@@ -34767,8 +34767,8 @@
       <c r="H32" s="30" t="s">
         <v>401</v>
       </c>
-      <c r="I32" s="30" t="s">
-        <v>402</v>
+      <c r="I32" s="20" t="s">
+        <v>405</v>
       </c>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
@@ -34912,7 +34912,7 @@
         <v>34.0</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E35" s="31" t="s">
         <v>302</v>
@@ -35453,7 +35453,7 @@
         <v>401</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J45" s="31"/>
       <c r="K45" s="31"/>
@@ -35655,7 +35655,7 @@
         <v>401</v>
       </c>
       <c r="I49" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J49" s="31"/>
       <c r="K49" s="31"/>
@@ -35811,7 +35811,7 @@
         <v>401</v>
       </c>
       <c r="I53" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J53" s="31"/>
       <c r="K53" s="31"/>
@@ -36013,7 +36013,7 @@
         <v>401</v>
       </c>
       <c r="I57" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J57" s="31"/>
       <c r="K57" s="31"/>
@@ -39909,7 +39909,7 @@
         <v>401</v>
       </c>
       <c r="I55" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J55" s="31"/>
       <c r="K55" s="31"/>
@@ -40069,7 +40069,7 @@
         <v>401</v>
       </c>
       <c r="I58" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J58" s="30"/>
       <c r="K58" s="30"/>
@@ -40229,7 +40229,7 @@
         <v>401</v>
       </c>
       <c r="I61" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J61" s="31"/>
       <c r="K61" s="31"/>
@@ -40389,7 +40389,7 @@
         <v>401</v>
       </c>
       <c r="I64" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J64" s="30"/>
       <c r="K64" s="30"/>
@@ -40549,7 +40549,7 @@
         <v>401</v>
       </c>
       <c r="I67" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K67" s="31"/>
       <c r="L67" s="31" t="s">
@@ -40707,7 +40707,7 @@
         <v>401</v>
       </c>
       <c r="I70" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K70" s="30"/>
       <c r="L70" s="30" t="s">
@@ -40866,7 +40866,7 @@
         <v>401</v>
       </c>
       <c r="I73" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K73" s="31"/>
       <c r="L73" s="31" t="s">
@@ -40961,7 +40961,7 @@
         <v>401</v>
       </c>
       <c r="I76" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K76" s="30"/>
       <c r="L76" s="30" t="s">
@@ -41110,7 +41110,7 @@
         <v>401</v>
       </c>
       <c r="I80" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K80" s="30"/>
       <c r="L80" s="30" t="s">

</xml_diff>